<commit_message>
Add data and gitignore file
</commit_message>
<xml_diff>
--- a/data/Price Development and Forecast PKO and Jet Fuel_values_sent.xlsx
+++ b/data/Price Development and Forecast PKO and Jet Fuel_values_sent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athanasioskaravangelis/Desktop/RSM BAM/Workshop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athanasioskaravangelis/Desktop/RSM BAM/Workshop/pko_forecasting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5316B2-7702-B44C-BA0A-B989CC5ABFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6B26C4-62A5-E642-A0C4-D5F60343A665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{AB45C537-59F9-4248-9665-B3FB2EA3726C}"/>
   </bookViews>
@@ -298,8 +298,52 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jeroen Beukeboom</author>
+  </authors>
+  <commentList>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{BB269E29-4054-B043-B1FB-D829085C56EE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jeroen Beukeboom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Ozlem confirmed 3,3x as conversion from $c/gallon
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="92">
   <si>
     <t>Oil World Report</t>
   </si>
@@ -572,6 +616,9 @@
   </si>
   <si>
     <t>Jet Fuel US US$/MT</t>
+  </si>
+  <si>
+    <t>Palmkernel oil(FOB Malaysia)</t>
   </si>
 </sst>
 </file>
@@ -11471,11 +11518,11 @@
   <dimension ref="B1:AP599"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C218" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="M186" activePane="bottomRight" state="frozen"/>
       <selection activeCell="EH5" sqref="EH5"/>
       <selection pane="topRight" activeCell="EH5" sqref="EH5"/>
       <selection pane="bottomLeft" activeCell="EH5" sqref="EH5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5:N221"/>
+      <selection pane="bottomRight" activeCell="V151" sqref="V151:V220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -39041,16 +39088,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E979B1DF-D953-E84E-B7CE-AE15FB733F89}">
-  <dimension ref="A1:M217"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E979B1DF-D953-E84E-B7CE-AE15FB733F89}">
+  <dimension ref="A1:Q217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>2</v>
@@ -39088,8 +39135,20 @@
       <c r="M1" s="105" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="N1" s="105" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="105" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="105" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
@@ -39103,8 +39162,11 @@
       <c r="K2" s="94"/>
       <c r="L2" s="94"/>
       <c r="M2" s="94"/>
-    </row>
-    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="23"/>
+    </row>
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>38718</v>
       </c>
@@ -39130,8 +39192,11 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>38749</v>
       </c>
@@ -39157,8 +39222,11 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
-    </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>38777</v>
       </c>
@@ -39184,8 +39252,11 @@
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
-    </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>38808</v>
       </c>
@@ -39211,8 +39282,11 @@
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17">
         <v>38838</v>
       </c>
@@ -39238,8 +39312,11 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
-    </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>38869</v>
       </c>
@@ -39265,8 +39342,11 @@
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
-    </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>38899</v>
       </c>
@@ -39292,8 +39372,11 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
-    </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>38930</v>
       </c>
@@ -39319,8 +39402,11 @@
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
-    </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>38961</v>
       </c>
@@ -39346,8 +39432,11 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
-    </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
         <v>38991</v>
       </c>
@@ -39373,8 +39462,11 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
-    </row>
-    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17">
         <v>39022</v>
       </c>
@@ -39400,8 +39492,11 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
-    </row>
-    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>39052</v>
       </c>
@@ -39427,8 +39522,11 @@
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
-    </row>
-    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17">
         <v>39083</v>
       </c>
@@ -39454,8 +39552,11 @@
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
-    </row>
-    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17">
         <v>39114</v>
       </c>
@@ -39481,8 +39582,11 @@
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
-    </row>
-    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
         <v>39142</v>
       </c>
@@ -39508,8 +39612,11 @@
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
-    </row>
-    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17">
         <v>39173</v>
       </c>
@@ -39535,8 +39642,11 @@
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
-    </row>
-    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17">
         <v>39203</v>
       </c>
@@ -39562,8 +39672,11 @@
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
-    </row>
-    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17">
         <v>39234</v>
       </c>
@@ -39589,8 +39702,11 @@
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
-    </row>
-    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17">
         <v>39264</v>
       </c>
@@ -39616,8 +39732,11 @@
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
-    </row>
-    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>39295</v>
       </c>
@@ -39643,8 +39762,11 @@
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
-    </row>
-    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <v>39326</v>
       </c>
@@ -39670,8 +39792,11 @@
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
-    </row>
-    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17">
         <v>39356</v>
       </c>
@@ -39697,8 +39822,11 @@
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
-    </row>
-    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17">
         <v>39387</v>
       </c>
@@ -39724,8 +39852,11 @@
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
-    </row>
-    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17">
         <v>39417</v>
       </c>
@@ -39751,8 +39882,11 @@
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
-    </row>
-    <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17">
         <v>39448</v>
       </c>
@@ -39780,8 +39914,11 @@
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
       <c r="M27" s="18"/>
-    </row>
-    <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17">
         <v>39479</v>
       </c>
@@ -39809,8 +39946,11 @@
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
-    </row>
-    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17">
         <v>39508</v>
       </c>
@@ -39838,8 +39978,11 @@
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
-    </row>
-    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17">
         <v>39539</v>
       </c>
@@ -39867,8 +40010,11 @@
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
-    </row>
-    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17">
         <v>39569</v>
       </c>
@@ -39896,8 +40042,11 @@
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
-    </row>
-    <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17">
         <v>39600</v>
       </c>
@@ -39925,8 +40074,11 @@
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
-    </row>
-    <row r="33" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17">
         <v>39630</v>
       </c>
@@ -39954,8 +40106,11 @@
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
-    </row>
-    <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17">
         <v>39661</v>
       </c>
@@ -39983,8 +40138,11 @@
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
-    </row>
-    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17">
         <v>39692</v>
       </c>
@@ -40012,8 +40170,11 @@
       <c r="K35" s="18"/>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
-    </row>
-    <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17">
         <v>39722</v>
       </c>
@@ -40041,8 +40202,11 @@
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
-    </row>
-    <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17">
         <v>39753</v>
       </c>
@@ -40070,8 +40234,11 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17">
         <v>39783</v>
       </c>
@@ -40099,8 +40266,11 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17">
         <v>39814</v>
       </c>
@@ -40128,8 +40298,11 @@
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
-    </row>
-    <row r="40" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17">
         <v>39845</v>
       </c>
@@ -40157,8 +40330,11 @@
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
-    </row>
-    <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="3"/>
+    </row>
+    <row r="41" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17">
         <v>39873</v>
       </c>
@@ -40186,8 +40362,11 @@
       <c r="K41" s="20"/>
       <c r="L41" s="20"/>
       <c r="M41" s="20"/>
-    </row>
-    <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="3"/>
+    </row>
+    <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17">
         <v>39904</v>
       </c>
@@ -40215,8 +40394,11 @@
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20"/>
-    </row>
-    <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17">
         <v>39934</v>
       </c>
@@ -40244,8 +40426,11 @@
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
       <c r="M43" s="20"/>
-    </row>
-    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="3"/>
+    </row>
+    <row r="44" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17">
         <v>39965</v>
       </c>
@@ -40273,8 +40458,11 @@
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
       <c r="M44" s="20"/>
-    </row>
-    <row r="45" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="3"/>
+    </row>
+    <row r="45" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17">
         <v>39995</v>
       </c>
@@ -40302,8 +40490,11 @@
       <c r="K45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="20"/>
-    </row>
-    <row r="46" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="106"/>
+    </row>
+    <row r="46" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17">
         <v>40026</v>
       </c>
@@ -40331,8 +40522,11 @@
       <c r="K46" s="20"/>
       <c r="L46" s="20"/>
       <c r="M46" s="20"/>
-    </row>
-    <row r="47" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N46" s="20"/>
+      <c r="O46" s="20"/>
+      <c r="P46" s="106"/>
+    </row>
+    <row r="47" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="17">
         <v>40057</v>
       </c>
@@ -40360,8 +40554,11 @@
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
       <c r="M47" s="20"/>
-    </row>
-    <row r="48" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="106"/>
+    </row>
+    <row r="48" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="17">
         <v>40087</v>
       </c>
@@ -40389,8 +40586,11 @@
       <c r="K48" s="20"/>
       <c r="L48" s="20"/>
       <c r="M48" s="20"/>
-    </row>
-    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="106"/>
+    </row>
+    <row r="49" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="17">
         <v>40118</v>
       </c>
@@ -40418,8 +40618,11 @@
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
       <c r="M49" s="20"/>
-    </row>
-    <row r="50" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="106"/>
+    </row>
+    <row r="50" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="17">
         <v>40148</v>
       </c>
@@ -40447,8 +40650,11 @@
       <c r="K50" s="20"/>
       <c r="L50" s="20"/>
       <c r="M50" s="20"/>
-    </row>
-    <row r="51" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="106"/>
+    </row>
+    <row r="51" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="17">
         <v>40179</v>
       </c>
@@ -40476,8 +40682,11 @@
       <c r="K51" s="20"/>
       <c r="L51" s="20"/>
       <c r="M51" s="20"/>
-    </row>
-    <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="106"/>
+    </row>
+    <row r="52" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="17">
         <v>40210</v>
       </c>
@@ -40505,8 +40714,11 @@
       <c r="K52" s="20"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
-    </row>
-    <row r="53" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="106"/>
+    </row>
+    <row r="53" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="17">
         <v>40238</v>
       </c>
@@ -40534,8 +40746,11 @@
       <c r="K53" s="20"/>
       <c r="L53" s="20"/>
       <c r="M53" s="20"/>
-    </row>
-    <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+      <c r="P53" s="3"/>
+    </row>
+    <row r="54" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="17">
         <v>40269</v>
       </c>
@@ -40563,8 +40778,11 @@
       <c r="K54" s="20"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20"/>
-    </row>
-    <row r="55" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="3"/>
+    </row>
+    <row r="55" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="17">
         <v>40299</v>
       </c>
@@ -40592,8 +40810,11 @@
       <c r="K55" s="20"/>
       <c r="L55" s="20"/>
       <c r="M55" s="20"/>
-    </row>
-    <row r="56" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="3"/>
+    </row>
+    <row r="56" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="17">
         <v>40330</v>
       </c>
@@ -40621,8 +40842,11 @@
       <c r="K56" s="20"/>
       <c r="L56" s="20"/>
       <c r="M56" s="20"/>
-    </row>
-    <row r="57" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N56" s="20"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="3"/>
+    </row>
+    <row r="57" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="17">
         <v>40360</v>
       </c>
@@ -40650,8 +40874,11 @@
       <c r="K57" s="20"/>
       <c r="L57" s="20"/>
       <c r="M57" s="20"/>
-    </row>
-    <row r="58" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N57" s="20"/>
+      <c r="O57" s="20"/>
+      <c r="P57" s="3"/>
+    </row>
+    <row r="58" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="17">
         <v>40391</v>
       </c>
@@ -40679,8 +40906,11 @@
       <c r="K58" s="20"/>
       <c r="L58" s="20"/>
       <c r="M58" s="20"/>
-    </row>
-    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="3"/>
+    </row>
+    <row r="59" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="17">
         <v>40422</v>
       </c>
@@ -40708,8 +40938,11 @@
       <c r="K59" s="20"/>
       <c r="L59" s="20"/>
       <c r="M59" s="20"/>
-    </row>
-    <row r="60" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N59" s="20"/>
+      <c r="O59" s="20"/>
+      <c r="P59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="17">
         <v>40452</v>
       </c>
@@ -40737,8 +40970,11 @@
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
       <c r="M60" s="20"/>
-    </row>
-    <row r="61" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="3"/>
+    </row>
+    <row r="61" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="17">
         <v>40483</v>
       </c>
@@ -40766,8 +41002,11 @@
       <c r="K61" s="20"/>
       <c r="L61" s="20"/>
       <c r="M61" s="20"/>
-    </row>
-    <row r="62" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="3"/>
+    </row>
+    <row r="62" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="17">
         <v>40513</v>
       </c>
@@ -40795,8 +41034,11 @@
       <c r="K62" s="20"/>
       <c r="L62" s="20"/>
       <c r="M62" s="20"/>
-    </row>
-    <row r="63" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="3"/>
+    </row>
+    <row r="63" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="17">
         <v>40544</v>
       </c>
@@ -40824,8 +41066,11 @@
       <c r="K63" s="20"/>
       <c r="L63" s="20"/>
       <c r="M63" s="20"/>
-    </row>
-    <row r="64" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N63" s="20"/>
+      <c r="O63" s="20"/>
+      <c r="P63" s="3"/>
+    </row>
+    <row r="64" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="17">
         <v>40575</v>
       </c>
@@ -40853,8 +41098,11 @@
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20"/>
-    </row>
-    <row r="65" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="3"/>
+    </row>
+    <row r="65" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="17">
         <v>40603</v>
       </c>
@@ -40882,8 +41130,11 @@
       <c r="K65" s="20"/>
       <c r="L65" s="20"/>
       <c r="M65" s="20"/>
-    </row>
-    <row r="66" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N65" s="20"/>
+      <c r="O65" s="20"/>
+      <c r="P65" s="3"/>
+    </row>
+    <row r="66" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="17">
         <v>40634</v>
       </c>
@@ -40911,8 +41162,11 @@
       <c r="K66" s="20"/>
       <c r="L66" s="20"/>
       <c r="M66" s="20"/>
-    </row>
-    <row r="67" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="3"/>
+    </row>
+    <row r="67" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="17">
         <v>40664</v>
       </c>
@@ -40940,8 +41194,11 @@
       <c r="K67" s="20"/>
       <c r="L67" s="20"/>
       <c r="M67" s="20"/>
-    </row>
-    <row r="68" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N67" s="20"/>
+      <c r="O67" s="20"/>
+      <c r="P67" s="3"/>
+    </row>
+    <row r="68" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="17">
         <v>40695</v>
       </c>
@@ -40969,8 +41226,11 @@
       <c r="K68" s="20"/>
       <c r="L68" s="20"/>
       <c r="M68" s="20"/>
-    </row>
-    <row r="69" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N68" s="20"/>
+      <c r="O68" s="20"/>
+      <c r="P68" s="3"/>
+    </row>
+    <row r="69" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="17">
         <v>40725</v>
       </c>
@@ -40998,8 +41258,11 @@
       <c r="K69" s="20"/>
       <c r="L69" s="20"/>
       <c r="M69" s="20"/>
-    </row>
-    <row r="70" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N69" s="20"/>
+      <c r="O69" s="20"/>
+      <c r="P69" s="3"/>
+    </row>
+    <row r="70" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="17">
         <v>40756</v>
       </c>
@@ -41027,8 +41290,11 @@
       <c r="K70" s="20"/>
       <c r="L70" s="20"/>
       <c r="M70" s="20"/>
-    </row>
-    <row r="71" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N70" s="20"/>
+      <c r="O70" s="20"/>
+      <c r="P70" s="3"/>
+    </row>
+    <row r="71" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="17">
         <v>40787</v>
       </c>
@@ -41056,8 +41322,11 @@
       <c r="K71" s="20"/>
       <c r="L71" s="20"/>
       <c r="M71" s="20"/>
-    </row>
-    <row r="72" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N71" s="20"/>
+      <c r="O71" s="20"/>
+      <c r="P71" s="3"/>
+    </row>
+    <row r="72" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="17">
         <v>40817</v>
       </c>
@@ -41085,8 +41354,11 @@
       <c r="K72" s="20"/>
       <c r="L72" s="20"/>
       <c r="M72" s="20"/>
-    </row>
-    <row r="73" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N72" s="20"/>
+      <c r="O72" s="20"/>
+      <c r="P72" s="3"/>
+    </row>
+    <row r="73" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="17">
         <v>40848</v>
       </c>
@@ -41114,8 +41386,11 @@
       <c r="K73" s="20"/>
       <c r="L73" s="20"/>
       <c r="M73" s="20"/>
-    </row>
-    <row r="74" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N73" s="20"/>
+      <c r="O73" s="20"/>
+      <c r="P73" s="3"/>
+    </row>
+    <row r="74" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="17">
         <v>40878</v>
       </c>
@@ -41143,8 +41418,11 @@
       <c r="K74" s="20"/>
       <c r="L74" s="20"/>
       <c r="M74" s="20"/>
-    </row>
-    <row r="75" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N74" s="20"/>
+      <c r="O74" s="20"/>
+      <c r="P74" s="3"/>
+    </row>
+    <row r="75" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="17">
         <v>40909</v>
       </c>
@@ -41172,8 +41450,11 @@
       <c r="K75" s="20"/>
       <c r="L75" s="20"/>
       <c r="M75" s="20"/>
-    </row>
-    <row r="76" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N75" s="20"/>
+      <c r="O75" s="20"/>
+      <c r="P75" s="24"/>
+    </row>
+    <row r="76" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="17">
         <v>40940</v>
       </c>
@@ -41201,8 +41482,11 @@
       <c r="K76" s="20"/>
       <c r="L76" s="20"/>
       <c r="M76" s="20"/>
-    </row>
-    <row r="77" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N76" s="20"/>
+      <c r="O76" s="20"/>
+      <c r="P76" s="24"/>
+    </row>
+    <row r="77" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="17">
         <v>40969</v>
       </c>
@@ -41230,8 +41514,11 @@
       <c r="K77" s="20"/>
       <c r="L77" s="20"/>
       <c r="M77" s="20"/>
-    </row>
-    <row r="78" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N77" s="20"/>
+      <c r="O77" s="20"/>
+      <c r="P77" s="24"/>
+    </row>
+    <row r="78" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="17">
         <v>41000</v>
       </c>
@@ -41259,8 +41546,11 @@
       <c r="K78" s="20"/>
       <c r="L78" s="20"/>
       <c r="M78" s="20"/>
-    </row>
-    <row r="79" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N78" s="20"/>
+      <c r="O78" s="20"/>
+      <c r="P78" s="24"/>
+    </row>
+    <row r="79" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="17">
         <v>41030</v>
       </c>
@@ -41288,8 +41578,11 @@
       <c r="K79" s="20"/>
       <c r="L79" s="20"/>
       <c r="M79" s="20"/>
-    </row>
-    <row r="80" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N79" s="20"/>
+      <c r="O79" s="20"/>
+      <c r="P79" s="24"/>
+    </row>
+    <row r="80" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="17">
         <v>41061</v>
       </c>
@@ -41317,8 +41610,11 @@
       <c r="K80" s="20"/>
       <c r="L80" s="20"/>
       <c r="M80" s="20"/>
-    </row>
-    <row r="81" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N80" s="20"/>
+      <c r="O80" s="20"/>
+      <c r="P80" s="24"/>
+    </row>
+    <row r="81" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="17">
         <v>41091</v>
       </c>
@@ -41346,8 +41642,11 @@
       <c r="K81" s="20"/>
       <c r="L81" s="20"/>
       <c r="M81" s="20"/>
-    </row>
-    <row r="82" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N81" s="20"/>
+      <c r="O81" s="20"/>
+      <c r="P81" s="24"/>
+    </row>
+    <row r="82" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="17">
         <v>41122</v>
       </c>
@@ -41375,8 +41674,11 @@
       <c r="K82" s="20"/>
       <c r="L82" s="20"/>
       <c r="M82" s="20"/>
-    </row>
-    <row r="83" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N82" s="20"/>
+      <c r="O82" s="20"/>
+      <c r="P82" s="24"/>
+    </row>
+    <row r="83" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="17">
         <v>41153</v>
       </c>
@@ -41404,8 +41706,11 @@
       <c r="K83" s="20"/>
       <c r="L83" s="20"/>
       <c r="M83" s="20"/>
-    </row>
-    <row r="84" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N83" s="20"/>
+      <c r="O83" s="20"/>
+      <c r="P83" s="24"/>
+    </row>
+    <row r="84" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="17">
         <v>41183</v>
       </c>
@@ -41433,8 +41738,11 @@
       <c r="K84" s="20"/>
       <c r="L84" s="20"/>
       <c r="M84" s="20"/>
-    </row>
-    <row r="85" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N84" s="20"/>
+      <c r="O84" s="20"/>
+      <c r="P84" s="24"/>
+    </row>
+    <row r="85" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="17">
         <v>41214</v>
       </c>
@@ -41462,8 +41770,11 @@
       <c r="K85" s="20"/>
       <c r="L85" s="20"/>
       <c r="M85" s="20"/>
-    </row>
-    <row r="86" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N85" s="20"/>
+      <c r="O85" s="20"/>
+      <c r="P85" s="24"/>
+    </row>
+    <row r="86" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="17">
         <v>41244</v>
       </c>
@@ -41491,8 +41802,11 @@
       <c r="K86" s="20"/>
       <c r="L86" s="20"/>
       <c r="M86" s="20"/>
-    </row>
-    <row r="87" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N86" s="20"/>
+      <c r="O86" s="20"/>
+      <c r="P86" s="24"/>
+    </row>
+    <row r="87" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="17">
         <v>41275</v>
       </c>
@@ -41520,8 +41834,11 @@
       <c r="K87" s="20"/>
       <c r="L87" s="20"/>
       <c r="M87" s="20"/>
-    </row>
-    <row r="88" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N87" s="20"/>
+      <c r="O87" s="20"/>
+      <c r="P87" s="24"/>
+    </row>
+    <row r="88" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="17">
         <v>41306</v>
       </c>
@@ -41549,8 +41866,11 @@
       <c r="K88" s="20"/>
       <c r="L88" s="20"/>
       <c r="M88" s="20"/>
-    </row>
-    <row r="89" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N88" s="20"/>
+      <c r="O88" s="20"/>
+      <c r="P88" s="3"/>
+    </row>
+    <row r="89" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="17">
         <v>41334</v>
       </c>
@@ -41578,8 +41898,11 @@
       <c r="K89" s="20"/>
       <c r="L89" s="20"/>
       <c r="M89" s="20"/>
-    </row>
-    <row r="90" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N89" s="20"/>
+      <c r="O89" s="20"/>
+      <c r="P89" s="3"/>
+    </row>
+    <row r="90" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="17">
         <v>41365</v>
       </c>
@@ -41607,8 +41930,11 @@
       <c r="K90" s="20"/>
       <c r="L90" s="20"/>
       <c r="M90" s="20"/>
-    </row>
-    <row r="91" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N90" s="20"/>
+      <c r="O90" s="20"/>
+      <c r="P90" s="24"/>
+    </row>
+    <row r="91" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="17">
         <v>41395</v>
       </c>
@@ -41636,8 +41962,11 @@
       <c r="K91" s="20"/>
       <c r="L91" s="20"/>
       <c r="M91" s="20"/>
-    </row>
-    <row r="92" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N91" s="20"/>
+      <c r="O91" s="20"/>
+      <c r="P91" s="24"/>
+    </row>
+    <row r="92" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="17">
         <v>41426</v>
       </c>
@@ -41665,8 +41994,11 @@
       <c r="K92" s="20"/>
       <c r="L92" s="20"/>
       <c r="M92" s="20"/>
-    </row>
-    <row r="93" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N92" s="20"/>
+      <c r="O92" s="20"/>
+      <c r="P92" s="24"/>
+    </row>
+    <row r="93" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="17">
         <v>41456</v>
       </c>
@@ -41694,8 +42026,11 @@
       <c r="K93" s="20"/>
       <c r="L93" s="20"/>
       <c r="M93" s="20"/>
-    </row>
-    <row r="94" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N93" s="20"/>
+      <c r="O93" s="20"/>
+      <c r="P93" s="24"/>
+    </row>
+    <row r="94" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="17">
         <v>41487</v>
       </c>
@@ -41723,8 +42058,11 @@
       <c r="K94" s="20"/>
       <c r="L94" s="20"/>
       <c r="M94" s="20"/>
-    </row>
-    <row r="95" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N94" s="20"/>
+      <c r="O94" s="20"/>
+      <c r="P94" s="24"/>
+    </row>
+    <row r="95" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="17">
         <v>41518</v>
       </c>
@@ -41752,8 +42090,11 @@
       <c r="K95" s="20"/>
       <c r="L95" s="20"/>
       <c r="M95" s="20"/>
-    </row>
-    <row r="96" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N95" s="20"/>
+      <c r="O95" s="20"/>
+      <c r="P95" s="24"/>
+    </row>
+    <row r="96" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="17">
         <v>41548</v>
       </c>
@@ -41781,8 +42122,11 @@
       <c r="K96" s="20"/>
       <c r="L96" s="20"/>
       <c r="M96" s="20"/>
-    </row>
-    <row r="97" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N96" s="20"/>
+      <c r="O96" s="20"/>
+      <c r="P96" s="24"/>
+    </row>
+    <row r="97" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="17">
         <v>41579</v>
       </c>
@@ -41810,8 +42154,11 @@
       <c r="K97" s="20"/>
       <c r="L97" s="20"/>
       <c r="M97" s="20"/>
-    </row>
-    <row r="98" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N97" s="20"/>
+      <c r="O97" s="20"/>
+      <c r="P97" s="24"/>
+    </row>
+    <row r="98" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="17">
         <v>41609</v>
       </c>
@@ -41839,8 +42186,11 @@
       <c r="K98" s="20"/>
       <c r="L98" s="20"/>
       <c r="M98" s="20"/>
-    </row>
-    <row r="99" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N98" s="20"/>
+      <c r="O98" s="20"/>
+      <c r="P98" s="24"/>
+    </row>
+    <row r="99" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="17">
         <v>41640</v>
       </c>
@@ -41868,8 +42218,11 @@
       <c r="K99" s="20"/>
       <c r="L99" s="20"/>
       <c r="M99" s="20"/>
-    </row>
-    <row r="100" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N99" s="20"/>
+      <c r="O99" s="20"/>
+      <c r="P99" s="24"/>
+    </row>
+    <row r="100" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="17">
         <v>41671</v>
       </c>
@@ -41897,8 +42250,11 @@
       <c r="K100" s="20"/>
       <c r="L100" s="20"/>
       <c r="M100" s="20"/>
-    </row>
-    <row r="101" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N100" s="20"/>
+      <c r="O100" s="20"/>
+      <c r="P100" s="3"/>
+    </row>
+    <row r="101" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="17">
         <v>41699</v>
       </c>
@@ -41926,8 +42282,11 @@
       <c r="K101" s="20"/>
       <c r="L101" s="20"/>
       <c r="M101" s="20"/>
-    </row>
-    <row r="102" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N101" s="20"/>
+      <c r="O101" s="20"/>
+      <c r="P101" s="3"/>
+    </row>
+    <row r="102" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="17">
         <v>41730</v>
       </c>
@@ -41955,8 +42314,11 @@
       <c r="K102" s="20"/>
       <c r="L102" s="20"/>
       <c r="M102" s="20"/>
-    </row>
-    <row r="103" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N102" s="20"/>
+      <c r="O102" s="20"/>
+      <c r="P102" s="24"/>
+    </row>
+    <row r="103" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="17">
         <v>41760</v>
       </c>
@@ -41984,8 +42346,11 @@
       <c r="K103" s="20"/>
       <c r="L103" s="20"/>
       <c r="M103" s="20"/>
-    </row>
-    <row r="104" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N103" s="20"/>
+      <c r="O103" s="20"/>
+      <c r="P103" s="24"/>
+    </row>
+    <row r="104" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="17">
         <v>41791</v>
       </c>
@@ -42013,8 +42378,11 @@
       <c r="K104" s="20"/>
       <c r="L104" s="20"/>
       <c r="M104" s="20"/>
-    </row>
-    <row r="105" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N104" s="20"/>
+      <c r="O104" s="20"/>
+      <c r="P104" s="24"/>
+    </row>
+    <row r="105" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="17">
         <v>41821</v>
       </c>
@@ -42042,8 +42410,11 @@
       <c r="K105" s="20"/>
       <c r="L105" s="20"/>
       <c r="M105" s="20"/>
-    </row>
-    <row r="106" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N105" s="20"/>
+      <c r="O105" s="20"/>
+      <c r="P105" s="24"/>
+    </row>
+    <row r="106" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="17">
         <v>41852</v>
       </c>
@@ -42071,8 +42442,11 @@
       <c r="K106" s="20"/>
       <c r="L106" s="20"/>
       <c r="M106" s="20"/>
-    </row>
-    <row r="107" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N106" s="20"/>
+      <c r="O106" s="20"/>
+      <c r="P106" s="24"/>
+    </row>
+    <row r="107" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="17">
         <v>41883</v>
       </c>
@@ -42100,8 +42474,11 @@
       <c r="K107" s="20"/>
       <c r="L107" s="20"/>
       <c r="M107" s="20"/>
-    </row>
-    <row r="108" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N107" s="20"/>
+      <c r="O107" s="20"/>
+      <c r="P107" s="24"/>
+    </row>
+    <row r="108" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="17">
         <v>41913</v>
       </c>
@@ -42129,8 +42506,11 @@
       <c r="K108" s="20"/>
       <c r="L108" s="20"/>
       <c r="M108" s="20"/>
-    </row>
-    <row r="109" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N108" s="20"/>
+      <c r="O108" s="20"/>
+      <c r="P108" s="24"/>
+    </row>
+    <row r="109" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="17">
         <v>41944</v>
       </c>
@@ -42158,8 +42538,11 @@
       <c r="K109" s="20"/>
       <c r="L109" s="20"/>
       <c r="M109" s="20"/>
-    </row>
-    <row r="110" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N109" s="20"/>
+      <c r="O109" s="20"/>
+      <c r="P109" s="24"/>
+    </row>
+    <row r="110" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="17">
         <v>41974</v>
       </c>
@@ -42187,8 +42570,11 @@
       <c r="K110" s="20"/>
       <c r="L110" s="20"/>
       <c r="M110" s="20"/>
-    </row>
-    <row r="111" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N110" s="20"/>
+      <c r="O110" s="20"/>
+      <c r="P110" s="24"/>
+    </row>
+    <row r="111" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="26">
         <v>42005</v>
       </c>
@@ -42222,8 +42608,18 @@
         <v>1245</v>
       </c>
       <c r="M111" s="92"/>
-    </row>
-    <row r="112" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N111" s="92">
+        <v>539.67999999999995</v>
+      </c>
+      <c r="O111" s="92">
+        <v>148.63999999999999</v>
+      </c>
+      <c r="P111" s="91">
+        <f t="shared" ref="P111:P174" si="0">O111*3.3</f>
+        <v>490.51199999999994</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="29">
         <v>42036</v>
       </c>
@@ -42257,8 +42653,18 @@
         <v>1245</v>
       </c>
       <c r="M112" s="92"/>
-    </row>
-    <row r="113" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N112" s="92">
+        <v>612.52499999999998</v>
+      </c>
+      <c r="O112" s="92">
+        <v>177.71250000000001</v>
+      </c>
+      <c r="P112" s="91">
+        <f t="shared" si="0"/>
+        <v>586.45124999999996</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="29">
         <v>42064</v>
       </c>
@@ -42292,8 +42698,18 @@
         <v>1245</v>
       </c>
       <c r="M113" s="92"/>
-    </row>
-    <row r="114" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N113" s="92">
+        <v>580.25</v>
+      </c>
+      <c r="O113" s="92">
+        <v>162.86000000000001</v>
+      </c>
+      <c r="P113" s="91">
+        <f t="shared" si="0"/>
+        <v>537.43799999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="29">
         <v>42095</v>
       </c>
@@ -42327,8 +42743,18 @@
         <v>1435</v>
       </c>
       <c r="M114" s="92"/>
-    </row>
-    <row r="115" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N114" s="92">
+        <v>582.29999999999995</v>
+      </c>
+      <c r="O114" s="92">
+        <v>169.03</v>
+      </c>
+      <c r="P114" s="91">
+        <f t="shared" si="0"/>
+        <v>557.79899999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="29">
         <v>42125</v>
       </c>
@@ -42362,8 +42788,18 @@
         <v>1435</v>
       </c>
       <c r="M115" s="92"/>
-    </row>
-    <row r="116" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N115" s="92">
+        <v>621.46</v>
+      </c>
+      <c r="O115" s="92">
+        <v>184.16249999999999</v>
+      </c>
+      <c r="P115" s="91">
+        <f t="shared" si="0"/>
+        <v>607.73624999999993</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="29">
         <v>42156</v>
       </c>
@@ -42397,8 +42833,18 @@
         <v>1435</v>
       </c>
       <c r="M116" s="92"/>
-    </row>
-    <row r="117" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N116" s="92">
+        <v>605.84</v>
+      </c>
+      <c r="O116" s="92">
+        <v>173.08</v>
+      </c>
+      <c r="P116" s="91">
+        <f t="shared" si="0"/>
+        <v>571.16399999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="29">
         <v>42186</v>
       </c>
@@ -42432,8 +42878,18 @@
         <v>1300</v>
       </c>
       <c r="M117" s="92"/>
-    </row>
-    <row r="118" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N117" s="92">
+        <v>539.54</v>
+      </c>
+      <c r="O117" s="92">
+        <v>154.02000000000001</v>
+      </c>
+      <c r="P117" s="91">
+        <f t="shared" si="0"/>
+        <v>508.26600000000002</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="29">
         <v>42217</v>
       </c>
@@ -42467,8 +42923,18 @@
         <v>1300</v>
       </c>
       <c r="M118" s="92"/>
-    </row>
-    <row r="119" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N118" s="92">
+        <v>478.07</v>
+      </c>
+      <c r="O118" s="92">
+        <v>139.03</v>
+      </c>
+      <c r="P118" s="91">
+        <f t="shared" si="0"/>
+        <v>458.79899999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="29">
         <v>42248</v>
       </c>
@@ -42502,8 +42968,18 @@
         <v>1300</v>
       </c>
       <c r="M119" s="92"/>
-    </row>
-    <row r="120" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N119" s="92">
+        <v>491.07</v>
+      </c>
+      <c r="O119" s="92">
+        <v>138.33000000000001</v>
+      </c>
+      <c r="P119" s="91">
+        <f t="shared" si="0"/>
+        <v>456.48900000000003</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="29">
         <v>42278</v>
       </c>
@@ -42537,8 +43013,18 @@
         <v>1150</v>
       </c>
       <c r="M120" s="92"/>
-    </row>
-    <row r="121" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N120" s="92">
+        <v>473.27</v>
+      </c>
+      <c r="O120" s="92">
+        <v>138.47999999999999</v>
+      </c>
+      <c r="P120" s="91">
+        <f t="shared" si="0"/>
+        <v>456.98399999999992</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="29">
         <v>42309</v>
       </c>
@@ -42572,8 +43058,18 @@
         <v>1150</v>
       </c>
       <c r="M121" s="92"/>
-    </row>
-    <row r="122" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N121" s="92">
+        <v>455.14</v>
+      </c>
+      <c r="O121" s="92">
+        <v>131.11000000000001</v>
+      </c>
+      <c r="P121" s="91">
+        <f t="shared" si="0"/>
+        <v>432.66300000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="29">
         <v>42339</v>
       </c>
@@ -42607,8 +43103,18 @@
         <v>1150</v>
       </c>
       <c r="M122" s="92"/>
-    </row>
-    <row r="123" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N122" s="92">
+        <v>383.61</v>
+      </c>
+      <c r="O122" s="92">
+        <v>106.49</v>
+      </c>
+      <c r="P122" s="91">
+        <f t="shared" si="0"/>
+        <v>351.41699999999997</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="29">
         <v>42370</v>
       </c>
@@ -42642,8 +43148,18 @@
         <v>1175</v>
       </c>
       <c r="M123" s="92"/>
-    </row>
-    <row r="124" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N123" s="92">
+        <v>313.9375</v>
+      </c>
+      <c r="O123" s="92">
+        <v>91.137500000000003</v>
+      </c>
+      <c r="P123" s="91">
+        <f t="shared" si="0"/>
+        <v>300.75374999999997</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="29">
         <v>42401</v>
       </c>
@@ -42677,8 +43193,18 @@
         <v>1175</v>
       </c>
       <c r="M124" s="92"/>
-    </row>
-    <row r="125" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N124" s="92">
+        <v>330.75</v>
+      </c>
+      <c r="O124" s="92">
+        <v>97.59</v>
+      </c>
+      <c r="P124" s="91">
+        <f t="shared" si="0"/>
+        <v>322.04699999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="29">
         <v>42430</v>
       </c>
@@ -42712,8 +43238,18 @@
         <v>1175</v>
       </c>
       <c r="M125" s="92"/>
-    </row>
-    <row r="126" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N125" s="92">
+        <v>376.68</v>
+      </c>
+      <c r="O125" s="92">
+        <v>107.42</v>
+      </c>
+      <c r="P125" s="91">
+        <f t="shared" si="0"/>
+        <v>354.48599999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="29">
         <v>42461</v>
       </c>
@@ -42747,8 +43283,18 @@
         <v>1600</v>
       </c>
       <c r="M126" s="92"/>
-    </row>
-    <row r="127" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N126" s="92">
+        <v>397.42</v>
+      </c>
+      <c r="O126" s="92">
+        <v>113.45</v>
+      </c>
+      <c r="P126" s="91">
+        <f t="shared" si="0"/>
+        <v>374.38499999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="29">
         <v>42491</v>
       </c>
@@ -42782,8 +43328,18 @@
         <v>1600</v>
       </c>
       <c r="M127" s="92"/>
-    </row>
-    <row r="128" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N127" s="92">
+        <v>443.5</v>
+      </c>
+      <c r="O127" s="92">
+        <v>129.53</v>
+      </c>
+      <c r="P127" s="91">
+        <f t="shared" si="0"/>
+        <v>427.44899999999996</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="29">
         <v>42522</v>
       </c>
@@ -42817,8 +43373,18 @@
         <v>1600</v>
       </c>
       <c r="M128" s="92"/>
-    </row>
-    <row r="129" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N128" s="92">
+        <v>466.95</v>
+      </c>
+      <c r="O128" s="92">
+        <v>137.93</v>
+      </c>
+      <c r="P128" s="91">
+        <f t="shared" si="0"/>
+        <v>455.16899999999998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="29">
         <v>42552</v>
       </c>
@@ -42852,8 +43418,18 @@
         <v>1675</v>
       </c>
       <c r="M129" s="92"/>
-    </row>
-    <row r="130" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N129" s="92">
+        <v>432.55</v>
+      </c>
+      <c r="O129" s="92">
+        <v>127.08</v>
+      </c>
+      <c r="P129" s="91">
+        <f t="shared" si="0"/>
+        <v>419.36399999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="29">
         <v>42583</v>
       </c>
@@ -42887,8 +43463,18 @@
         <v>1675</v>
       </c>
       <c r="M130" s="92"/>
-    </row>
-    <row r="131" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N130" s="92">
+        <v>435.37</v>
+      </c>
+      <c r="O130" s="92">
+        <v>129.22</v>
+      </c>
+      <c r="P130" s="91">
+        <f t="shared" si="0"/>
+        <v>426.42599999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="29">
         <v>42614</v>
       </c>
@@ -42922,8 +43508,18 @@
         <v>1675</v>
       </c>
       <c r="M131" s="92"/>
-    </row>
-    <row r="132" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N131" s="92">
+        <v>442.87</v>
+      </c>
+      <c r="O131" s="92">
+        <v>131.72</v>
+      </c>
+      <c r="P131" s="91">
+        <f t="shared" si="0"/>
+        <v>434.67599999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="29">
         <v>42644</v>
       </c>
@@ -42957,8 +43553,18 @@
         <v>2075</v>
       </c>
       <c r="M132" s="92"/>
-    </row>
-    <row r="133" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N132" s="92">
+        <v>485.81</v>
+      </c>
+      <c r="O132" s="92">
+        <v>145.72</v>
+      </c>
+      <c r="P132" s="91">
+        <f t="shared" si="0"/>
+        <v>480.87599999999998</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="29">
         <v>42675</v>
       </c>
@@ -42992,8 +43598,18 @@
         <v>2075</v>
       </c>
       <c r="M133" s="92"/>
-    </row>
-    <row r="134" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N133" s="92">
+        <v>454.73</v>
+      </c>
+      <c r="O133" s="92">
+        <v>135.51</v>
+      </c>
+      <c r="P133" s="91">
+        <f t="shared" si="0"/>
+        <v>447.18299999999994</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="29">
         <v>42705</v>
       </c>
@@ -43027,8 +43643,18 @@
         <v>2075</v>
       </c>
       <c r="M134" s="92"/>
-    </row>
-    <row r="135" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N134" s="92">
+        <v>512.17999999999995</v>
+      </c>
+      <c r="O134" s="92">
+        <v>149.55000000000001</v>
+      </c>
+      <c r="P134" s="91">
+        <f t="shared" si="0"/>
+        <v>493.51499999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="29">
         <v>42736</v>
       </c>
@@ -43064,8 +43690,18 @@
         <v>2450</v>
       </c>
       <c r="M135" s="92"/>
-    </row>
-    <row r="136" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N135" s="92">
+        <v>518.74</v>
+      </c>
+      <c r="O135" s="92">
+        <v>150.51</v>
+      </c>
+      <c r="P135" s="91">
+        <f t="shared" si="0"/>
+        <v>496.68299999999994</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="29">
         <v>42767</v>
       </c>
@@ -43101,8 +43737,18 @@
         <v>2450</v>
       </c>
       <c r="M136" s="92"/>
-    </row>
-    <row r="137" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N136" s="92">
+        <v>525.33749999999998</v>
+      </c>
+      <c r="O136" s="92">
+        <v>154.54374999999999</v>
+      </c>
+      <c r="P136" s="91">
+        <f t="shared" si="0"/>
+        <v>509.99437499999993</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="29">
         <v>42795</v>
       </c>
@@ -43138,8 +43784,18 @@
         <v>2450</v>
       </c>
       <c r="M137" s="92"/>
-    </row>
-    <row r="138" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N137" s="92">
+        <v>494.06</v>
+      </c>
+      <c r="O137" s="92">
+        <v>144.47</v>
+      </c>
+      <c r="P137" s="91">
+        <f t="shared" si="0"/>
+        <v>476.75099999999998</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="29">
         <v>42826</v>
       </c>
@@ -43175,8 +43831,18 @@
         <v>1935</v>
       </c>
       <c r="M138" s="92"/>
-    </row>
-    <row r="139" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N138" s="92">
+        <v>507.67</v>
+      </c>
+      <c r="O138" s="92">
+        <v>150.55000000000001</v>
+      </c>
+      <c r="P138" s="91">
+        <f t="shared" si="0"/>
+        <v>496.815</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="29">
         <v>42856</v>
       </c>
@@ -43212,8 +43878,18 @@
         <v>1935</v>
       </c>
       <c r="M139" s="92"/>
-    </row>
-    <row r="140" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N139" s="92">
+        <v>485.2</v>
+      </c>
+      <c r="O139" s="92">
+        <v>140.88</v>
+      </c>
+      <c r="P139" s="91">
+        <f t="shared" si="0"/>
+        <v>464.90399999999994</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="29">
         <v>42887</v>
       </c>
@@ -43249,8 +43925,18 @@
         <v>1935</v>
       </c>
       <c r="M140" s="92"/>
-    </row>
-    <row r="141" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N140" s="92">
+        <v>457.43</v>
+      </c>
+      <c r="O140" s="92">
+        <v>129.35</v>
+      </c>
+      <c r="P140" s="91">
+        <f t="shared" si="0"/>
+        <v>426.85499999999996</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="29">
         <v>42917</v>
       </c>
@@ -43286,8 +43972,18 @@
         <v>1700</v>
       </c>
       <c r="M141" s="92"/>
-    </row>
-    <row r="142" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N141" s="92">
+        <v>484.58</v>
+      </c>
+      <c r="O141" s="92">
+        <v>141.93</v>
+      </c>
+      <c r="P141" s="91">
+        <f t="shared" si="0"/>
+        <v>468.36899999999997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="29">
         <v>42948</v>
       </c>
@@ -43323,8 +44019,18 @@
         <v>1700</v>
       </c>
       <c r="M142" s="92"/>
-    </row>
-    <row r="143" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N142" s="92">
+        <v>515.02</v>
+      </c>
+      <c r="O142" s="92">
+        <v>156.07</v>
+      </c>
+      <c r="P142" s="91">
+        <f t="shared" si="0"/>
+        <v>515.03099999999995</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="29">
         <v>42979</v>
       </c>
@@ -43360,8 +44066,18 @@
         <v>1700</v>
       </c>
       <c r="M143" s="92"/>
-    </row>
-    <row r="144" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N143" s="92">
+        <v>557.12</v>
+      </c>
+      <c r="O143" s="92">
+        <v>180.89</v>
+      </c>
+      <c r="P143" s="91">
+        <f t="shared" si="0"/>
+        <v>596.9369999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="29">
         <v>43009</v>
       </c>
@@ -43397,8 +44113,18 @@
         <v>1975</v>
       </c>
       <c r="M144" s="92"/>
-    </row>
-    <row r="145" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N144" s="92">
+        <v>557.09</v>
+      </c>
+      <c r="O144" s="92">
+        <v>165.55</v>
+      </c>
+      <c r="P144" s="91">
+        <f t="shared" si="0"/>
+        <v>546.31500000000005</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="29">
         <v>43040</v>
       </c>
@@ -43434,8 +44160,18 @@
         <v>1975</v>
       </c>
       <c r="M145" s="92"/>
-    </row>
-    <row r="146" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N145" s="92">
+        <v>605.01</v>
+      </c>
+      <c r="O145" s="92">
+        <v>175.98</v>
+      </c>
+      <c r="P145" s="91">
+        <f t="shared" si="0"/>
+        <v>580.73399999999992</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="29">
         <v>43070</v>
       </c>
@@ -43471,8 +44207,18 @@
         <v>1975</v>
       </c>
       <c r="M146" s="93"/>
-    </row>
-    <row r="147" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N146" s="93">
+        <v>611.25</v>
+      </c>
+      <c r="O146" s="93">
+        <v>181.625</v>
+      </c>
+      <c r="P146" s="91">
+        <f t="shared" si="0"/>
+        <v>599.36249999999995</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="29">
         <v>43101</v>
       </c>
@@ -43508,8 +44254,21 @@
         <v>1875</v>
       </c>
       <c r="M147" s="92"/>
-    </row>
-    <row r="148" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N147" s="92">
+        <v>654.88</v>
+      </c>
+      <c r="O147" s="92">
+        <v>195.22</v>
+      </c>
+      <c r="P147" s="91">
+        <f t="shared" si="0"/>
+        <v>644.226</v>
+      </c>
+      <c r="Q147" s="4">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="29">
         <v>43132</v>
       </c>
@@ -43545,8 +44304,21 @@
         <v>1875</v>
       </c>
       <c r="M148" s="92"/>
-    </row>
-    <row r="149" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N148" s="92">
+        <v>640.42499999999995</v>
+      </c>
+      <c r="O148" s="92">
+        <v>185.3125</v>
+      </c>
+      <c r="P148" s="91">
+        <f t="shared" si="0"/>
+        <v>611.53125</v>
+      </c>
+      <c r="Q148" s="4">
+        <v>1145.3800000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="29">
         <v>43160</v>
       </c>
@@ -43582,8 +44354,21 @@
         <v>1875</v>
       </c>
       <c r="M149" s="92"/>
-    </row>
-    <row r="150" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N149" s="92">
+        <v>641.85</v>
+      </c>
+      <c r="O149" s="92">
+        <v>185.11</v>
+      </c>
+      <c r="P149" s="91">
+        <f t="shared" si="0"/>
+        <v>610.86300000000006</v>
+      </c>
+      <c r="Q149" s="4">
+        <v>1016.19</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="29">
         <v>43191</v>
       </c>
@@ -43619,8 +44404,21 @@
         <v>1525</v>
       </c>
       <c r="M150" s="92"/>
-    </row>
-    <row r="151" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N150" s="92">
+        <v>691.49</v>
+      </c>
+      <c r="O150" s="92">
+        <v>201.49</v>
+      </c>
+      <c r="P150" s="91">
+        <f t="shared" si="0"/>
+        <v>664.91700000000003</v>
+      </c>
+      <c r="Q150" s="4">
+        <v>1006.71</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="29">
         <v>43221</v>
       </c>
@@ -43656,8 +44454,21 @@
         <v>1525</v>
       </c>
       <c r="M151" s="92"/>
-    </row>
-    <row r="152" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N151" s="92">
+        <v>728.07</v>
+      </c>
+      <c r="O151" s="92">
+        <v>215.48</v>
+      </c>
+      <c r="P151" s="91">
+        <f t="shared" si="0"/>
+        <v>711.08399999999995</v>
+      </c>
+      <c r="Q151" s="4">
+        <v>935.25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="29">
         <v>43252</v>
       </c>
@@ -43693,8 +44504,21 @@
         <v>1525</v>
       </c>
       <c r="M152" s="92"/>
-    </row>
-    <row r="153" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N152" s="92">
+        <v>702.71</v>
+      </c>
+      <c r="O152" s="92">
+        <v>208.67</v>
+      </c>
+      <c r="P152" s="91">
+        <f t="shared" si="0"/>
+        <v>688.61099999999988</v>
+      </c>
+      <c r="Q152" s="4">
+        <v>865.71</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="29">
         <v>43282</v>
       </c>
@@ -43730,8 +44554,21 @@
         <v>1325</v>
       </c>
       <c r="M153" s="92"/>
-    </row>
-    <row r="154" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N153" s="92">
+        <v>702.85</v>
+      </c>
+      <c r="O153" s="92">
+        <v>209.85</v>
+      </c>
+      <c r="P153" s="91">
+        <f t="shared" si="0"/>
+        <v>692.505</v>
+      </c>
+      <c r="Q153" s="4">
+        <v>877.16</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="29">
         <v>43313</v>
       </c>
@@ -43767,8 +44604,21 @@
         <v>1325</v>
       </c>
       <c r="M154" s="92"/>
-    </row>
-    <row r="155" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N154" s="92">
+        <v>697.63</v>
+      </c>
+      <c r="O154" s="92">
+        <v>211.74</v>
+      </c>
+      <c r="P154" s="91">
+        <f t="shared" si="0"/>
+        <v>698.74199999999996</v>
+      </c>
+      <c r="Q154" s="4">
+        <v>900.22</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="29">
         <v>43344</v>
       </c>
@@ -43804,8 +44654,21 @@
         <v>1325</v>
       </c>
       <c r="M155" s="92"/>
-    </row>
-    <row r="156" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N155" s="92">
+        <v>731.54375000000005</v>
+      </c>
+      <c r="O155" s="92">
+        <v>218.61250000000001</v>
+      </c>
+      <c r="P155" s="91">
+        <f t="shared" si="0"/>
+        <v>721.42124999999999</v>
+      </c>
+      <c r="Q155" s="4">
+        <v>865.63</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="29">
         <v>43374</v>
       </c>
@@ -43841,8 +44704,21 @@
         <v>1425</v>
       </c>
       <c r="M156" s="92"/>
-    </row>
-    <row r="157" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N156" s="92">
+        <v>768.91</v>
+      </c>
+      <c r="O156" s="92">
+        <v>224.77</v>
+      </c>
+      <c r="P156" s="91">
+        <f t="shared" si="0"/>
+        <v>741.74099999999999</v>
+      </c>
+      <c r="Q156" s="4">
+        <v>794.49</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="29">
         <v>43405</v>
       </c>
@@ -43878,8 +44754,21 @@
         <v>1425</v>
       </c>
       <c r="M157" s="92"/>
-    </row>
-    <row r="158" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N157" s="92">
+        <v>671.1875</v>
+      </c>
+      <c r="O157" s="92">
+        <v>194.74</v>
+      </c>
+      <c r="P157" s="91">
+        <f t="shared" si="0"/>
+        <v>642.64199999999994</v>
+      </c>
+      <c r="Q157" s="4">
+        <v>707.62</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="29">
         <v>43435</v>
       </c>
@@ -43915,8 +44804,21 @@
         <v>1425</v>
       </c>
       <c r="M158" s="92"/>
-    </row>
-    <row r="159" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N158" s="92">
+        <v>594.01</v>
+      </c>
+      <c r="O158" s="92">
+        <v>171.44</v>
+      </c>
+      <c r="P158" s="91">
+        <f t="shared" si="0"/>
+        <v>565.75199999999995</v>
+      </c>
+      <c r="Q158" s="4">
+        <v>738.36</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="29">
         <v>43466</v>
       </c>
@@ -43952,8 +44854,21 @@
         <v>1375</v>
       </c>
       <c r="M159" s="92"/>
-    </row>
-    <row r="160" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N159" s="92">
+        <v>602.20000000000005</v>
+      </c>
+      <c r="O159" s="92">
+        <v>179.84</v>
+      </c>
+      <c r="P159" s="91">
+        <f t="shared" si="0"/>
+        <v>593.47199999999998</v>
+      </c>
+      <c r="Q159" s="4">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="29">
         <v>43497</v>
       </c>
@@ -43989,8 +44904,21 @@
         <v>1375</v>
       </c>
       <c r="M160" s="92"/>
-    </row>
-    <row r="161" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N160" s="92">
+        <v>632.03750000000002</v>
+      </c>
+      <c r="O160" s="92">
+        <v>190.49375000000001</v>
+      </c>
+      <c r="P160" s="91">
+        <f t="shared" si="0"/>
+        <v>628.62937499999998</v>
+      </c>
+      <c r="Q160" s="4">
+        <v>694.67</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="29">
         <v>43525</v>
       </c>
@@ -44026,8 +44954,21 @@
         <v>1375</v>
       </c>
       <c r="M161" s="92"/>
-    </row>
-    <row r="162" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N161" s="92">
+        <v>645</v>
+      </c>
+      <c r="O161" s="92">
+        <v>190.46</v>
+      </c>
+      <c r="P161" s="91">
+        <f t="shared" si="0"/>
+        <v>628.51800000000003</v>
+      </c>
+      <c r="Q161" s="4">
+        <v>654.72</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="29">
         <v>43556</v>
       </c>
@@ -44063,8 +45004,21 @@
         <v>1225</v>
       </c>
       <c r="M162" s="92"/>
-    </row>
-    <row r="163" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N162" s="92">
+        <v>662.82500000000005</v>
+      </c>
+      <c r="O162" s="92">
+        <v>197.5</v>
+      </c>
+      <c r="P162" s="91">
+        <f t="shared" si="0"/>
+        <v>651.75</v>
+      </c>
+      <c r="Q162" s="4">
+        <v>636.23</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="29">
         <v>43586</v>
       </c>
@@ -44100,8 +45054,21 @@
         <v>1225</v>
       </c>
       <c r="M163" s="92"/>
-    </row>
-    <row r="164" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N163" s="92">
+        <v>666.97</v>
+      </c>
+      <c r="O163" s="92">
+        <v>197.14</v>
+      </c>
+      <c r="P163" s="91">
+        <f t="shared" si="0"/>
+        <v>650.5619999999999</v>
+      </c>
+      <c r="Q163" s="4">
+        <v>573.36</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="29">
         <v>43617</v>
       </c>
@@ -44137,8 +45104,21 @@
         <v>1225</v>
       </c>
       <c r="M164" s="92"/>
-    </row>
-    <row r="165" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N164" s="92">
+        <v>611.48749999999995</v>
+      </c>
+      <c r="O164" s="92">
+        <v>181.33125000000001</v>
+      </c>
+      <c r="P164" s="91">
+        <f t="shared" si="0"/>
+        <v>598.39312500000005</v>
+      </c>
+      <c r="Q164" s="4">
+        <v>542.24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="29">
         <v>43647</v>
       </c>
@@ -44174,8 +45154,21 @@
         <v>1125</v>
       </c>
       <c r="M165" s="92"/>
-    </row>
-    <row r="166" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N165" s="92">
+        <v>640.22</v>
+      </c>
+      <c r="O165" s="92">
+        <v>190.7</v>
+      </c>
+      <c r="P165" s="91">
+        <f t="shared" si="0"/>
+        <v>629.30999999999995</v>
+      </c>
+      <c r="Q165" s="4">
+        <v>555.03</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="29">
         <v>43678</v>
       </c>
@@ -44211,8 +45204,21 @@
         <v>1125</v>
       </c>
       <c r="M166" s="92"/>
-    </row>
-    <row r="167" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N166" s="92">
+        <v>605.91999999999996</v>
+      </c>
+      <c r="O166" s="92">
+        <v>179.76</v>
+      </c>
+      <c r="P166" s="91">
+        <f t="shared" si="0"/>
+        <v>593.20799999999997</v>
+      </c>
+      <c r="Q166" s="4">
+        <v>619.33000000000004</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="29">
         <v>43709</v>
       </c>
@@ -44248,8 +45254,21 @@
         <v>1125</v>
       </c>
       <c r="M167" s="92"/>
-    </row>
-    <row r="168" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N167" s="92">
+        <v>640.375</v>
+      </c>
+      <c r="O167" s="92">
+        <v>187.32</v>
+      </c>
+      <c r="P167" s="91">
+        <f t="shared" si="0"/>
+        <v>618.15599999999995</v>
+      </c>
+      <c r="Q167" s="4">
+        <v>613.15</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="29">
         <v>43739</v>
       </c>
@@ -44285,8 +45304,21 @@
         <v>1030</v>
       </c>
       <c r="M168" s="92"/>
-    </row>
-    <row r="169" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N168" s="92">
+        <v>628.72</v>
+      </c>
+      <c r="O168" s="92">
+        <v>186.32</v>
+      </c>
+      <c r="P168" s="91">
+        <f t="shared" si="0"/>
+        <v>614.85599999999999</v>
+      </c>
+      <c r="Q168" s="4">
+        <v>593.74</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="29">
         <v>43770</v>
       </c>
@@ -44322,8 +45354,21 @@
         <v>1030</v>
       </c>
       <c r="M169" s="92"/>
-    </row>
-    <row r="170" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N169" s="92">
+        <v>620.27</v>
+      </c>
+      <c r="O169" s="92">
+        <v>182.05</v>
+      </c>
+      <c r="P169" s="91">
+        <f t="shared" si="0"/>
+        <v>600.76499999999999</v>
+      </c>
+      <c r="Q169" s="4">
+        <v>755.76</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="29">
         <v>43800</v>
       </c>
@@ -44359,8 +45404,21 @@
         <v>1030</v>
       </c>
       <c r="M170" s="92"/>
-    </row>
-    <row r="171" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N170" s="92">
+        <v>635.9</v>
+      </c>
+      <c r="O170" s="92">
+        <v>187.625</v>
+      </c>
+      <c r="P170" s="91">
+        <f t="shared" si="0"/>
+        <v>619.16250000000002</v>
+      </c>
+      <c r="Q170" s="4">
+        <v>944.7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="29">
         <v>43831</v>
       </c>
@@ -44396,8 +45454,21 @@
         <v>1305</v>
       </c>
       <c r="M171" s="92"/>
-    </row>
-    <row r="172" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N171" s="92">
+        <v>609.79999999999995</v>
+      </c>
+      <c r="O171" s="92">
+        <v>176.78</v>
+      </c>
+      <c r="P171" s="91">
+        <f t="shared" si="0"/>
+        <v>583.37400000000002</v>
+      </c>
+      <c r="Q171" s="4">
+        <v>954.7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="29">
         <v>43862</v>
       </c>
@@ -44433,8 +45504,21 @@
         <v>1305</v>
       </c>
       <c r="M172" s="92"/>
-    </row>
-    <row r="173" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N172" s="92">
+        <v>524.03750000000002</v>
+      </c>
+      <c r="O172" s="92">
+        <v>151.32499999999999</v>
+      </c>
+      <c r="P172" s="91">
+        <f t="shared" si="0"/>
+        <v>499.37249999999995</v>
+      </c>
+      <c r="Q172" s="4">
+        <v>801.84</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="29">
         <v>43891</v>
       </c>
@@ -44470,8 +45554,21 @@
         <v>1305</v>
       </c>
       <c r="M173" s="92"/>
-    </row>
-    <row r="174" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N173" s="92">
+        <v>324.14999999999998</v>
+      </c>
+      <c r="O173" s="92">
+        <v>95.3</v>
+      </c>
+      <c r="P173" s="91">
+        <f t="shared" si="0"/>
+        <v>314.48999999999995</v>
+      </c>
+      <c r="Q173" s="4">
+        <v>691.04</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="29">
         <v>43922</v>
       </c>
@@ -44507,8 +45604,21 @@
         <v>1200</v>
       </c>
       <c r="M174" s="92"/>
-    </row>
-    <row r="175" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N174" s="92">
+        <v>183.66249999999999</v>
+      </c>
+      <c r="O174" s="92">
+        <v>56.306249999999999</v>
+      </c>
+      <c r="P174" s="91">
+        <f t="shared" si="0"/>
+        <v>185.81062499999999</v>
+      </c>
+      <c r="Q174" s="4">
+        <v>720.69</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="29">
         <v>43952</v>
       </c>
@@ -44544,8 +45654,21 @@
         <v>1200</v>
       </c>
       <c r="M175" s="92"/>
-    </row>
-    <row r="176" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N175" s="92">
+        <v>216.42500000000001</v>
+      </c>
+      <c r="O175" s="92">
+        <v>66.362499999999997</v>
+      </c>
+      <c r="P175" s="91">
+        <f t="shared" ref="P175:P217" si="1">O175*3.3</f>
+        <v>218.99624999999997</v>
+      </c>
+      <c r="Q175" s="4">
+        <v>684.95</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="29">
         <v>43983</v>
       </c>
@@ -44581,8 +45704,21 @@
         <v>1200</v>
       </c>
       <c r="M176" s="92"/>
-    </row>
-    <row r="177" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N176" s="92">
+        <v>320.94</v>
+      </c>
+      <c r="O176" s="92">
+        <v>98.53</v>
+      </c>
+      <c r="P176" s="91">
+        <f t="shared" si="1"/>
+        <v>325.149</v>
+      </c>
+      <c r="Q176" s="4">
+        <v>724.62</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="29">
         <v>44013</v>
       </c>
@@ -44618,8 +45754,21 @@
         <v>1140</v>
       </c>
       <c r="M177" s="92"/>
-    </row>
-    <row r="178" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N177" s="92">
+        <v>347.99</v>
+      </c>
+      <c r="O177" s="92">
+        <v>108.72</v>
+      </c>
+      <c r="P177" s="91">
+        <f t="shared" si="1"/>
+        <v>358.77599999999995</v>
+      </c>
+      <c r="Q177" s="4">
+        <v>683.93</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="29">
         <v>44044</v>
       </c>
@@ -44655,8 +45804,21 @@
         <v>1140</v>
       </c>
       <c r="M178" s="92"/>
-    </row>
-    <row r="179" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N178" s="92">
+        <v>347.49</v>
+      </c>
+      <c r="O178" s="92">
+        <v>108.91</v>
+      </c>
+      <c r="P178" s="91">
+        <f t="shared" si="1"/>
+        <v>359.40299999999996</v>
+      </c>
+      <c r="Q178" s="4">
+        <v>739.17</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="29">
         <v>44075</v>
       </c>
@@ -44692,8 +45854,21 @@
         <v>1140</v>
       </c>
       <c r="M179" s="92"/>
-    </row>
-    <row r="180" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N179" s="92">
+        <v>312.52999999999997</v>
+      </c>
+      <c r="O179" s="92">
+        <v>97.8</v>
+      </c>
+      <c r="P179" s="91">
+        <f t="shared" si="1"/>
+        <v>322.73999999999995</v>
+      </c>
+      <c r="Q179" s="4">
+        <v>767.84</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="29">
         <v>44105</v>
       </c>
@@ -44729,8 +45904,21 @@
         <v>1160</v>
       </c>
       <c r="M180" s="92"/>
-    </row>
-    <row r="181" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N180" s="92">
+        <v>331.53</v>
+      </c>
+      <c r="O180" s="92">
+        <v>100.05</v>
+      </c>
+      <c r="P180" s="91">
+        <f t="shared" si="1"/>
+        <v>330.16499999999996</v>
+      </c>
+      <c r="Q180" s="4">
+        <v>805.91</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="29">
         <v>44136</v>
       </c>
@@ -44766,8 +45954,21 @@
         <v>1160</v>
       </c>
       <c r="M181" s="92"/>
-    </row>
-    <row r="182" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N181" s="92">
+        <v>362.12</v>
+      </c>
+      <c r="O181" s="92">
+        <v>110.48</v>
+      </c>
+      <c r="P181" s="91">
+        <f t="shared" si="1"/>
+        <v>364.584</v>
+      </c>
+      <c r="Q181" s="4">
+        <v>1073.48</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="29">
         <v>44166</v>
       </c>
@@ -44803,8 +46004,21 @@
         <v>1160</v>
       </c>
       <c r="M182" s="92"/>
-    </row>
-    <row r="183" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N182" s="92">
+        <v>429.51</v>
+      </c>
+      <c r="O182" s="92">
+        <v>129.18</v>
+      </c>
+      <c r="P182" s="91">
+        <f t="shared" si="1"/>
+        <v>426.29399999999998</v>
+      </c>
+      <c r="Q182" s="4">
+        <v>1224.8699999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="29">
         <v>44197</v>
       </c>
@@ -44840,8 +46054,21 @@
         <v>1700</v>
       </c>
       <c r="M183" s="92"/>
-    </row>
-    <row r="184" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N183" s="92">
+        <v>469.00625000000002</v>
+      </c>
+      <c r="O183" s="92">
+        <v>142.91249999999999</v>
+      </c>
+      <c r="P183" s="91">
+        <f t="shared" si="1"/>
+        <v>471.61124999999998</v>
+      </c>
+      <c r="Q183" s="4">
+        <v>1368.31</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="29">
         <v>44228</v>
       </c>
@@ -44877,8 +46104,21 @@
         <v>1700</v>
       </c>
       <c r="M184" s="92"/>
-    </row>
-    <row r="185" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N184" s="92">
+        <v>521.875</v>
+      </c>
+      <c r="O184" s="92">
+        <v>163.44999999999999</v>
+      </c>
+      <c r="P184" s="91">
+        <f t="shared" si="1"/>
+        <v>539.38499999999988</v>
+      </c>
+      <c r="Q184" s="4">
+        <v>1353.68</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="29">
         <v>44256</v>
       </c>
@@ -44914,8 +46154,21 @@
         <v>1700</v>
       </c>
       <c r="M185" s="92"/>
-    </row>
-    <row r="186" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N185" s="92">
+        <v>539.6</v>
+      </c>
+      <c r="O185" s="92">
+        <v>169.875</v>
+      </c>
+      <c r="P185" s="91">
+        <f t="shared" si="1"/>
+        <v>560.58749999999998</v>
+      </c>
+      <c r="Q185" s="4">
+        <v>1478.07</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="29">
         <v>44287</v>
       </c>
@@ -44953,8 +46206,21 @@
       <c r="M186" s="92">
         <v>127.5</v>
       </c>
-    </row>
-    <row r="187" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N186" s="92">
+        <v>537.67499999999995</v>
+      </c>
+      <c r="O186" s="92">
+        <v>166.55</v>
+      </c>
+      <c r="P186" s="91">
+        <f t="shared" si="1"/>
+        <v>549.61500000000001</v>
+      </c>
+      <c r="Q186" s="4">
+        <v>1487.14</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="29">
         <v>44317</v>
       </c>
@@ -44992,8 +46258,21 @@
       <c r="M187" s="92">
         <v>137.5</v>
       </c>
-    </row>
-    <row r="188" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N187" s="92">
+        <v>574.71875</v>
+      </c>
+      <c r="O187" s="92">
+        <v>175.36875000000001</v>
+      </c>
+      <c r="P187" s="91">
+        <f t="shared" si="1"/>
+        <v>578.71687499999996</v>
+      </c>
+      <c r="Q187" s="4">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="29">
         <v>44348</v>
       </c>
@@ -45031,8 +46310,21 @@
       <c r="M188" s="92">
         <v>150.5</v>
       </c>
-    </row>
-    <row r="189" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N188" s="92">
+        <v>611.37</v>
+      </c>
+      <c r="O188" s="92">
+        <v>185.85</v>
+      </c>
+      <c r="P188" s="91">
+        <f t="shared" si="1"/>
+        <v>613.30499999999995</v>
+      </c>
+      <c r="Q188" s="4">
+        <v>1400.45</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="29">
         <v>44378</v>
       </c>
@@ -45070,8 +46362,21 @@
       <c r="M189" s="92">
         <v>155</v>
       </c>
-    </row>
-    <row r="190" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N189" s="92">
+        <v>623.67999999999995</v>
+      </c>
+      <c r="O189" s="92">
+        <v>189.82</v>
+      </c>
+      <c r="P189" s="91">
+        <f t="shared" si="1"/>
+        <v>626.40599999999995</v>
+      </c>
+      <c r="Q189" s="4">
+        <v>1270.5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="29">
         <v>44409</v>
       </c>
@@ -45109,8 +46414,21 @@
       <c r="M190" s="92">
         <v>155</v>
       </c>
-    </row>
-    <row r="191" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N190" s="92">
+        <v>605.21</v>
+      </c>
+      <c r="O190" s="92">
+        <v>182.03</v>
+      </c>
+      <c r="P190" s="91">
+        <f t="shared" si="1"/>
+        <v>600.69899999999996</v>
+      </c>
+      <c r="Q190" s="4">
+        <v>1333.44</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="29">
         <v>44440</v>
       </c>
@@ -45148,8 +46466,21 @@
       <c r="M191" s="92">
         <v>175</v>
       </c>
-    </row>
-    <row r="192" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N191" s="92">
+        <v>652.52</v>
+      </c>
+      <c r="O191" s="92">
+        <v>200.06</v>
+      </c>
+      <c r="P191" s="91">
+        <f t="shared" si="1"/>
+        <v>660.19799999999998</v>
+      </c>
+      <c r="Q191" s="4">
+        <v>1427.27</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="29">
         <v>44470</v>
       </c>
@@ -45187,8 +46518,21 @@
       <c r="M192" s="92">
         <v>257.5</v>
       </c>
-    </row>
-    <row r="193" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N192" s="92">
+        <v>754</v>
+      </c>
+      <c r="O192" s="92">
+        <v>229.875</v>
+      </c>
+      <c r="P192" s="91">
+        <f t="shared" si="1"/>
+        <v>758.58749999999998</v>
+      </c>
+      <c r="Q192" s="4">
+        <v>1807.25</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="29">
         <v>44501</v>
       </c>
@@ -45226,8 +46570,21 @@
       <c r="M193" s="92">
         <v>310</v>
       </c>
-    </row>
-    <row r="194" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N193" s="92">
+        <v>720.3125</v>
+      </c>
+      <c r="O193" s="92">
+        <v>219.19</v>
+      </c>
+      <c r="P193" s="91">
+        <f t="shared" si="1"/>
+        <v>723.327</v>
+      </c>
+      <c r="Q193" s="4">
+        <v>2068.61</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="29">
         <v>44531</v>
       </c>
@@ -45265,8 +46622,21 @@
       <c r="M194" s="92">
         <v>297.5</v>
       </c>
-    </row>
-    <row r="195" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N194" s="92">
+        <v>671.18</v>
+      </c>
+      <c r="O194" s="92">
+        <v>207.7</v>
+      </c>
+      <c r="P194" s="91">
+        <f t="shared" si="1"/>
+        <v>685.41</v>
+      </c>
+      <c r="Q194" s="4">
+        <v>1861.43</v>
+      </c>
+    </row>
+    <row r="195" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="29">
         <v>44562</v>
       </c>
@@ -45304,8 +46674,21 @@
       <c r="M195" s="92">
         <v>286.25</v>
       </c>
-    </row>
-    <row r="196" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N195" s="92">
+        <v>798.6875</v>
+      </c>
+      <c r="O195" s="92">
+        <v>246.125</v>
+      </c>
+      <c r="P195" s="91">
+        <f t="shared" si="1"/>
+        <v>812.21249999999998</v>
+      </c>
+      <c r="Q195" s="4">
+        <v>2195.79</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="29">
         <v>44593</v>
       </c>
@@ -45343,8 +46726,21 @@
       <c r="M196" s="92">
         <v>293.75</v>
       </c>
-    </row>
-    <row r="197" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N196" s="92">
+        <v>870.92499999999995</v>
+      </c>
+      <c r="O196" s="92">
+        <v>267.60624999999999</v>
+      </c>
+      <c r="P196" s="91">
+        <f t="shared" si="1"/>
+        <v>883.10062499999992</v>
+      </c>
+      <c r="Q196" s="4">
+        <v>2442.63</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="29">
         <v>44621</v>
       </c>
@@ -45382,8 +46778,21 @@
       <c r="M197" s="92">
         <v>307</v>
       </c>
-    </row>
-    <row r="198" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N197" s="92">
+        <v>1166.68</v>
+      </c>
+      <c r="O197" s="92">
+        <v>351.57</v>
+      </c>
+      <c r="P197" s="91">
+        <f t="shared" si="1"/>
+        <v>1160.1809999999998</v>
+      </c>
+      <c r="Q197" s="4">
+        <v>2441.48</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="29">
         <v>44652</v>
       </c>
@@ -45421,8 +46830,21 @@
       <c r="M198" s="92">
         <v>315</v>
       </c>
-    </row>
-    <row r="199" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N198" s="92">
+        <v>1214</v>
+      </c>
+      <c r="O198" s="92">
+        <v>393.97</v>
+      </c>
+      <c r="P198" s="91">
+        <f t="shared" si="1"/>
+        <v>1300.1010000000001</v>
+      </c>
+      <c r="Q198" s="4">
+        <v>2064.31</v>
+      </c>
+    </row>
+    <row r="199" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="29">
         <v>44682</v>
       </c>
@@ -45460,8 +46882,21 @@
       <c r="M199" s="92">
         <v>315</v>
       </c>
-    </row>
-    <row r="200" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N199" s="92">
+        <v>1271</v>
+      </c>
+      <c r="O199" s="92">
+        <v>386.91874999999999</v>
+      </c>
+      <c r="P199" s="91">
+        <f t="shared" si="1"/>
+        <v>1276.8318749999999</v>
+      </c>
+      <c r="Q199" s="4">
+        <v>1811.19</v>
+      </c>
+    </row>
+    <row r="200" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="29">
         <v>44713</v>
       </c>
@@ -45499,8 +46934,21 @@
       <c r="M200" s="92">
         <v>316</v>
       </c>
-    </row>
-    <row r="201" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N200" s="92">
+        <v>1417.4875</v>
+      </c>
+      <c r="O200" s="92">
+        <v>412.84</v>
+      </c>
+      <c r="P200" s="91">
+        <f t="shared" si="1"/>
+        <v>1362.3719999999998</v>
+      </c>
+      <c r="Q200" s="4">
+        <v>1554.5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="29">
         <v>44743</v>
       </c>
@@ -45538,8 +46986,21 @@
       <c r="M201" s="92">
         <v>342.5</v>
       </c>
-    </row>
-    <row r="202" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N201" s="92">
+        <v>1186.08</v>
+      </c>
+      <c r="O201" s="92">
+        <v>347.75</v>
+      </c>
+      <c r="P201" s="91">
+        <f t="shared" si="1"/>
+        <v>1147.575</v>
+      </c>
+      <c r="Q201" s="4">
+        <v>1301.05</v>
+      </c>
+    </row>
+    <row r="202" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="29">
         <v>44774</v>
       </c>
@@ -45577,8 +47038,21 @@
       <c r="M202" s="92">
         <v>345</v>
       </c>
-    </row>
-    <row r="203" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N202" s="92">
+        <v>1128.68</v>
+      </c>
+      <c r="O202" s="92">
+        <v>333.23</v>
+      </c>
+      <c r="P202" s="91">
+        <f t="shared" si="1"/>
+        <v>1099.6590000000001</v>
+      </c>
+      <c r="Q202" s="4">
+        <v>1173.04</v>
+      </c>
+    </row>
+    <row r="203" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="29">
         <v>44805</v>
       </c>
@@ -45616,8 +47090,21 @@
       <c r="M203" s="92">
         <v>345</v>
       </c>
-    </row>
-    <row r="204" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N203" s="92">
+        <v>1061.76</v>
+      </c>
+      <c r="O203" s="92">
+        <v>326.82</v>
+      </c>
+      <c r="P203" s="91">
+        <f t="shared" si="1"/>
+        <v>1078.5059999999999</v>
+      </c>
+      <c r="Q203" s="4">
+        <v>1249.29</v>
+      </c>
+    </row>
+    <row r="204" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="29">
         <v>44835</v>
       </c>
@@ -45655,8 +47142,21 @@
       <c r="M204" s="92">
         <v>325</v>
       </c>
-    </row>
-    <row r="205" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N204" s="92">
+        <v>1102.18</v>
+      </c>
+      <c r="O204" s="92">
+        <v>371.29</v>
+      </c>
+      <c r="P204" s="91">
+        <f t="shared" si="1"/>
+        <v>1225.2570000000001</v>
+      </c>
+      <c r="Q204" s="4">
+        <v>1038.81</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="29">
         <v>44866</v>
       </c>
@@ -45694,8 +47194,21 @@
       <c r="M205" s="92">
         <v>325</v>
       </c>
-    </row>
-    <row r="206" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N205" s="92">
+        <v>1042.82</v>
+      </c>
+      <c r="O205" s="92">
+        <v>318.16250000000002</v>
+      </c>
+      <c r="P205" s="91">
+        <f t="shared" si="1"/>
+        <v>1049.93625</v>
+      </c>
+      <c r="Q205" s="4">
+        <v>1061.58</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="29">
         <v>44896</v>
       </c>
@@ -45733,8 +47246,21 @@
       <c r="M206" s="92">
         <v>325</v>
       </c>
-    </row>
-    <row r="207" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N206" s="92">
+        <v>953.65</v>
+      </c>
+      <c r="O206" s="92">
+        <v>283.89999999999998</v>
+      </c>
+      <c r="P206" s="91">
+        <f t="shared" si="1"/>
+        <v>936.86999999999989</v>
+      </c>
+      <c r="Q206" s="4">
+        <v>1067.05</v>
+      </c>
+    </row>
+    <row r="207" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="29">
         <v>44927</v>
       </c>
@@ -45772,8 +47298,21 @@
       <c r="M207" s="92">
         <v>325</v>
       </c>
-    </row>
-    <row r="208" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N207" s="92">
+        <v>1009.58</v>
+      </c>
+      <c r="O207" s="92">
+        <v>353.3</v>
+      </c>
+      <c r="P207" s="91">
+        <f t="shared" si="1"/>
+        <v>1165.8899999999999</v>
+      </c>
+      <c r="Q207" s="4">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="208" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="29">
         <v>44958</v>
       </c>
@@ -45811,8 +47350,21 @@
       <c r="M208" s="92">
         <v>317.5</v>
       </c>
-    </row>
-    <row r="209" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N208" s="92">
+        <v>894.67499999999995</v>
+      </c>
+      <c r="O208" s="92">
+        <v>278.94</v>
+      </c>
+      <c r="P208" s="91">
+        <f t="shared" si="1"/>
+        <v>920.50199999999995</v>
+      </c>
+      <c r="Q208" s="4">
+        <v>1036.67</v>
+      </c>
+    </row>
+    <row r="209" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="29">
         <v>44986</v>
       </c>
@@ -45850,8 +47402,21 @@
       <c r="M209" s="92">
         <v>309</v>
       </c>
-    </row>
-    <row r="210" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N209" s="92">
+        <v>834.95</v>
+      </c>
+      <c r="O209" s="92">
+        <v>269.52</v>
+      </c>
+      <c r="P209" s="91">
+        <f t="shared" si="1"/>
+        <v>889.41599999999994</v>
+      </c>
+      <c r="Q209" s="4">
+        <v>1051.75</v>
+      </c>
+    </row>
+    <row r="210" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="29">
         <v>45017</v>
       </c>
@@ -45889,8 +47454,21 @@
       <c r="M210" s="92">
         <v>282.5</v>
       </c>
-    </row>
-    <row r="211" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N210" s="92">
+        <v>794.89</v>
+      </c>
+      <c r="O210" s="92">
+        <v>236.81</v>
+      </c>
+      <c r="P210" s="91">
+        <f t="shared" si="1"/>
+        <v>781.47299999999996</v>
+      </c>
+      <c r="Q210" s="4">
+        <v>1016.84</v>
+      </c>
+    </row>
+    <row r="211" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="29">
         <v>45047</v>
       </c>
@@ -45928,8 +47506,21 @@
       <c r="M211" s="92">
         <v>271</v>
       </c>
-    </row>
-    <row r="212" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N211" s="92">
+        <v>730.15</v>
+      </c>
+      <c r="O211" s="92">
+        <v>216.98750000000001</v>
+      </c>
+      <c r="P211" s="91">
+        <f t="shared" si="1"/>
+        <v>716.05875000000003</v>
+      </c>
+      <c r="Q211" s="4">
+        <v>992.5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="29">
         <v>45078</v>
       </c>
@@ -45967,8 +47558,21 @@
       <c r="M212" s="92">
         <v>267.5</v>
       </c>
-    </row>
-    <row r="213" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N212" s="92">
+        <v>746.18</v>
+      </c>
+      <c r="O212" s="92">
+        <v>225.71</v>
+      </c>
+      <c r="P212" s="91">
+        <f t="shared" si="1"/>
+        <v>744.84299999999996</v>
+      </c>
+      <c r="Q212" s="4">
+        <v>927.95</v>
+      </c>
+    </row>
+    <row r="213" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="29">
         <v>45108</v>
       </c>
@@ -46006,8 +47610,21 @@
       <c r="M213" s="92">
         <v>258.75</v>
       </c>
-    </row>
-    <row r="214" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N213" s="92">
+        <v>837.08</v>
+      </c>
+      <c r="O213" s="92">
+        <v>248.5</v>
+      </c>
+      <c r="P213" s="91">
+        <f t="shared" si="1"/>
+        <v>820.05</v>
+      </c>
+      <c r="Q213" s="4">
+        <v>998.1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="29">
         <v>45139</v>
       </c>
@@ -46045,8 +47662,21 @@
       <c r="M214" s="92">
         <v>233</v>
       </c>
-    </row>
-    <row r="215" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N214" s="92">
+        <v>974.74</v>
+      </c>
+      <c r="O214" s="92">
+        <v>298.82</v>
+      </c>
+      <c r="P214" s="91">
+        <f t="shared" si="1"/>
+        <v>986.10599999999988</v>
+      </c>
+      <c r="Q214" s="4">
+        <v>998.41</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="29">
         <v>45170</v>
       </c>
@@ -46084,8 +47714,21 @@
       <c r="M215" s="92">
         <v>230</v>
       </c>
-    </row>
-    <row r="216" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N215" s="92">
+        <v>1037.52</v>
+      </c>
+      <c r="O215" s="92">
+        <v>313.00625000000002</v>
+      </c>
+      <c r="P215" s="91">
+        <f t="shared" si="1"/>
+        <v>1032.920625</v>
+      </c>
+      <c r="Q215" s="4">
+        <v>957.64</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="29">
         <v>45200</v>
       </c>
@@ -46123,8 +47766,21 @@
       <c r="M216" s="31">
         <v>220</v>
       </c>
-    </row>
-    <row r="217" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N216" s="92">
+        <v>973.625</v>
+      </c>
+      <c r="O216" s="92">
+        <v>288.89999999999998</v>
+      </c>
+      <c r="P216" s="91">
+        <f t="shared" si="1"/>
+        <v>953.36999999999989</v>
+      </c>
+      <c r="Q216" s="4">
+        <v>912.38</v>
+      </c>
+    </row>
+    <row r="217" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="29">
         <v>45231</v>
       </c>
@@ -46162,8 +47818,21 @@
       <c r="M217" s="31">
         <v>220</v>
       </c>
+      <c r="N217" s="92">
+        <f t="shared" ref="N217" si="2">O217/O216*N216</f>
+        <v>957.1114572516442</v>
+      </c>
+      <c r="O217" s="92">
+        <v>284</v>
+      </c>
+      <c r="P217" s="91">
+        <f t="shared" si="1"/>
+        <v>937.19999999999993</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>